<commit_message>
fix: alterar método acp para 32 variáveis
</commit_message>
<xml_diff>
--- a/data/variables/variables.xlsx
+++ b/data/variables/variables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Váriáveis novas </t>
   </si>
@@ -21,75 +21,141 @@
     <t xml:space="preserve">name </t>
   </si>
   <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>Concórdia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6, 5, 1, 12, 8, 11, 14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Densidade Demográfica</t>
   </si>
   <si>
     <t xml:space="preserve">% de população urbana</t>
   </si>
   <si>
+    <t>Seara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17, 32</t>
+  </si>
+  <si>
     <t xml:space="preserve">% de pessoas em domicílios com energia elétrica 2010</t>
   </si>
   <si>
+    <t xml:space="preserve">N° Estabelecimentos de saúde</t>
+  </si>
+  <si>
     <t xml:space="preserve">`% da população em domicílios com água encanada 2010</t>
   </si>
   <si>
-    <t xml:space="preserve">N° Estabelecimentos de saúde</t>
-  </si>
-  <si>
     <t xml:space="preserve">N°de leitos em  estabelecimentos de saúde</t>
   </si>
   <si>
+    <t xml:space="preserve">Xavantina, C. Branco, Peritiba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23, 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">População economicamente ativa de 18 anos ou mais de idade 2010</t>
+  </si>
+  <si>
+    <t>Receitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peritiba, Lindoia, ipumirim</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taxa de analfabetismo - 15 anos ou mais de idade 2010</t>
   </si>
   <si>
-    <t xml:space="preserve">População economicamente ativa de 18 anos ou mais de idade 2010</t>
+    <t xml:space="preserve">VAB Serviços </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAB Industria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ipira, arabuta</t>
   </si>
   <si>
     <t xml:space="preserve">Taxa de desocupação - 18 anos ou mais de idade 2010</t>
   </si>
   <si>
+    <t xml:space="preserve">VAB Agropecuária</t>
+  </si>
+  <si>
     <t xml:space="preserve">PIB percapta</t>
   </si>
   <si>
-    <t>Receitas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAB Serviços </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAB Industria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAB Agropecuária</t>
+    <t xml:space="preserve">% de 25 anos ou mais de idade com ensino superior completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto bela vista, jaborá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24, 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% dos ocupados com ensino médio completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% dos ocupados com ensino superior completo</t>
+  </si>
+  <si>
+    <t>irani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% de ocupados de 18 anos ou mais de idade que são empregados com carteira</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>itá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26, 27</t>
   </si>
   <si>
     <t xml:space="preserve">Mortalidade infantil 2010</t>
   </si>
   <si>
+    <t>+</t>
+  </si>
+  <si>
     <t>IDMH</t>
   </si>
   <si>
     <t>IG</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t xml:space="preserve">% de pessoas em domicílios urbanos com coleta de lixo 2010</t>
   </si>
   <si>
     <t xml:space="preserve">% de 6 a 17 anos de idade na escola</t>
   </si>
   <si>
-    <t xml:space="preserve">% de 25 anos ou mais de idade com ensino superior completo</t>
+    <t xml:space="preserve">Índice de Theil-L dos rendimentos do trabalho - 18 anos ou mais de idade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendimento médio dos ocupados</t>
   </si>
   <si>
     <t xml:space="preserve">Taxa de frequência bruta ao ensino básico</t>
   </si>
   <si>
+    <t>g3</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Taxa de envelhecimento</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de Theil-L dos rendimentos do trabalho - 18 anos ou mais de idade</t>
-  </si>
-  <si>
     <t xml:space="preserve">% de pobres</t>
   </si>
   <si>
@@ -102,26 +168,20 @@
     <t xml:space="preserve">Renda per capita dos vulneráveis à pobreza</t>
   </si>
   <si>
-    <t xml:space="preserve">% dos ocupados com ensino médio completo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% dos ocupados com ensino superior completo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% de ocupados de 18 anos ou mais de idade que são empregados com carteira</t>
+    <t>g4</t>
   </si>
   <si>
     <t xml:space="preserve">% de ocupados de 18 anos ou mais de idade que são empregados sem carteira</t>
   </si>
   <si>
-    <t xml:space="preserve">Rendimento médio dos ocupados</t>
+    <t xml:space="preserve">15, 10, 09 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -129,11 +189,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="14.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Liberation Sans"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +209,35 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0"/>
+        <bgColor theme="7" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0"/>
+        <bgColor theme="8" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0"/>
+        <bgColor theme="5" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0"/>
+        <bgColor theme="9" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,15 +245,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="1" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,266 +810,493 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="67.28125"/>
+    <col bestFit="1" min="1" max="1" style="1" width="67.28125"/>
+    <col min="3" max="3" style="1" width="9.140625"/>
+    <col bestFit="1" min="4" max="4" width="68.921875"/>
+    <col bestFit="1" min="7" max="7" width="26.25390625"/>
+    <col bestFit="1" min="8" max="8" width="17.8515625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
+    <row r="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="10">
+        <v>22</v>
+      </c>
+      <c r="I9" s="11">
+        <v>19</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" t="s">
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="10">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" t="s">
+      <c r="D15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="12">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" t="s">
-        <v>17</v>
+      <c r="A17" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="12">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="12">
         <v>18</v>
       </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
+        <v>41</v>
+      </c>
+      <c r="B20" s="7">
         <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75">
+      <c r="A22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1">
         <v>21</v>
       </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
+      <c r="C22" s="1"/>
+      <c r="D22" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="8">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="12">
         <v>23</v>
       </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
+        <v>47</v>
+      </c>
+      <c r="B25" s="8">
         <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
+        <v>48</v>
+      </c>
+      <c r="B26" s="8">
         <v>25</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
+        <v>49</v>
+      </c>
+      <c r="B27" s="8">
         <v>26</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="8">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" ht="18.75">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -936,10 +1304,64 @@
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33">
+        <v>43</v>
+      </c>
+      <c r="B33" s="12">
         <v>32</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" ht="14.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" ht="14.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" ht="14.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" ht="14.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>